<commit_message>
Olwen CC2500 files added
</commit_message>
<xml_diff>
--- a/NeldeCalma/Calma calculations.xlsx
+++ b/NeldeCalma/Calma calculations.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
   <si>
     <t>LEDs power calculations</t>
   </si>
@@ -88,6 +88,18 @@
   </si>
   <si>
     <t>kHz</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>Ohm</t>
+  </si>
+  <si>
+    <t>U r max</t>
+  </si>
+  <si>
+    <t>I max</t>
   </si>
 </sst>
 </file>
@@ -759,10 +771,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C3"/>
+  <dimension ref="A2:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -791,6 +803,40 @@
       </c>
       <c r="C3" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="2">
+        <v>75</v>
+      </c>
+      <c r="C7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="2">
+        <v>2480</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="9">
+        <f>B8/B7</f>
+        <v>33.06666666666667</v>
+      </c>
+      <c r="C9" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
NeldeCalma modified: data transmission works, with periodic sleep enabled.
</commit_message>
<xml_diff>
--- a/NeldeCalma/Calma calculations.xlsx
+++ b/NeldeCalma/Calma calculations.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9114"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="210" windowWidth="18960" windowHeight="8415" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="210" windowWidth="18960" windowHeight="8415" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
     <sheet name="PWM" sheetId="2" r:id="rId2"/>
-    <sheet name="Лист3" sheetId="3" r:id="rId3"/>
+    <sheet name="Radio" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144315"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="43">
   <si>
     <t>LEDs power calculations</t>
   </si>
@@ -100,13 +100,61 @@
   </si>
   <si>
     <t>I max</t>
+  </si>
+  <si>
+    <t>Bitrate</t>
+  </si>
+  <si>
+    <t>Bit/s</t>
+  </si>
+  <si>
+    <t>Bit duration</t>
+  </si>
+  <si>
+    <t>uS</t>
+  </si>
+  <si>
+    <t>Byte duration</t>
+  </si>
+  <si>
+    <t>Experimental</t>
+  </si>
+  <si>
+    <t>mS</t>
+  </si>
+  <si>
+    <t>Packet duration</t>
+  </si>
+  <si>
+    <t>Receive duration</t>
+  </si>
+  <si>
+    <t>ms</t>
+  </si>
+  <si>
+    <t>*2</t>
+  </si>
+  <si>
+    <t>RX_OFF duration</t>
+  </si>
+  <si>
+    <t>RX_ON duration</t>
+  </si>
+  <si>
+    <t>ON/OFF ratio</t>
+  </si>
+  <si>
+    <t>%</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -157,8 +205,16 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -184,6 +240,11 @@
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
       </patternFill>
     </fill>
   </fills>
@@ -257,15 +318,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2"/>
@@ -278,9 +340,12 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="4"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="5" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="6"/>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="2" xfId="4" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
     <cellStyle name="20% - Accent3" xfId="5" builtinId="38"/>
+    <cellStyle name="Accent1" xfId="6" builtinId="29"/>
     <cellStyle name="Calculation" xfId="4" builtinId="22"/>
     <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -773,7 +838,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -846,12 +911,118 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A3:D14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3">
+        <v>10000</v>
+      </c>
+      <c r="C3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4">
+        <f>1000000/B3</f>
+        <v>100</v>
+      </c>
+      <c r="C4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5">
+        <f>B4*8</f>
+        <v>800</v>
+      </c>
+      <c r="C5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="2">
+        <v>24</v>
+      </c>
+      <c r="C9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="9">
+        <f>B9*2</f>
+        <v>48</v>
+      </c>
+      <c r="C10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="2">
+        <v>216</v>
+      </c>
+      <c r="C12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="2">
+        <v>54</v>
+      </c>
+      <c r="C13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="13">
+        <f>100*B13/(B13+B12)</f>
+        <v>20</v>
+      </c>
+      <c r="C14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Olwen: added color table
</commit_message>
<xml_diff>
--- a/NeldeCalma/Calma calculations.xlsx
+++ b/NeldeCalma/Calma calculations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9114"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="210" windowWidth="18960" windowHeight="8415" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="210" windowWidth="18960" windowHeight="8415" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="52">
   <si>
     <t>LEDs power calculations</t>
   </si>
@@ -145,6 +145,33 @@
   </si>
   <si>
     <t>%</t>
+  </si>
+  <si>
+    <t>Colors</t>
+  </si>
+  <si>
+    <t>RED_PWM_MAX</t>
+  </si>
+  <si>
+    <t>GREEN_PWM_MAX</t>
+  </si>
+  <si>
+    <t>BLUE_PWM_MAX</t>
+  </si>
+  <si>
+    <t>COLOR_STEP</t>
+  </si>
+  <si>
+    <t>Red variations</t>
+  </si>
+  <si>
+    <t>Green variations</t>
+  </si>
+  <si>
+    <t>Blue variations</t>
+  </si>
+  <si>
+    <t>Colors count</t>
   </si>
 </sst>
 </file>
@@ -327,7 +354,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2"/>
@@ -342,6 +369,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="5"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="6"/>
     <xf numFmtId="164" fontId="5" fillId="4" borderId="2" xfId="4" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="3"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="20% - Accent3" xfId="5" builtinId="38"/>
@@ -836,10 +864,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C9"/>
+  <dimension ref="A2:C20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -904,6 +932,79 @@
         <v>9</v>
       </c>
     </row>
+    <row r="12" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="14">
+        <f>B13/$B$16</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" s="14">
+        <f t="shared" ref="B18:B19" si="0">B14/$B$16</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" s="14">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" s="9">
+        <f>B19*B18*B17</f>
+        <v>8000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -913,7 +1014,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>

</xml_diff>